<commit_message>
add handguards and stocks
</commit_message>
<xml_diff>
--- a/changes/hk416-handguards.xlsx
+++ b/changes/hk416-handguards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifan/Documents/deadline-balancing/changes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F919B08-761F-476D-867E-6204A2F992AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21BD6DA-A372-2A47-9F0C-2372E9A53C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>new</t>
   </si>
@@ -80,28 +80,70 @@
     <t>price</t>
   </si>
   <si>
-    <t>hk_quad_rail_handguard</t>
-  </si>
-  <si>
-    <t>HK416A5 Quad Rail Handguard</t>
-  </si>
-  <si>
-    <t>mi_hk416_mlok_14i</t>
-  </si>
-  <si>
-    <t>Midwest Industries HK416 14" MLOK Handguard</t>
-  </si>
-  <si>
-    <t>mi_hk416_mlok_9i</t>
-  </si>
-  <si>
-    <t>Midwest Industries HK416 9" MLOK Handguard</t>
-  </si>
-  <si>
-    <t>hk_extended_quad_rail_handguard</t>
-  </si>
-  <si>
-    <t>HK416A5 Extended Quad Rail Handguard</t>
+    <t>kf_416_9i_quad_rail_handguard</t>
+  </si>
+  <si>
+    <t>kf_416_9i_quad_rail_handguard_with_flip_up_sight</t>
+  </si>
+  <si>
+    <t>kf_416_standard_length_quad_rail_handguard</t>
+  </si>
+  <si>
+    <t>kf_416_extended_length_quad_rail_handguard</t>
+  </si>
+  <si>
+    <t>kf_416_dmr_extra_long_handguard</t>
+  </si>
+  <si>
+    <t>kf_416c_handguard</t>
+  </si>
+  <si>
+    <t>kf_416_short_hkey_handguard</t>
+  </si>
+  <si>
+    <t>kf_416_14.5i_qd_mlok_handguard</t>
+  </si>
+  <si>
+    <t>f_416_long_qd_hkey_handguard</t>
+  </si>
+  <si>
+    <t>kf_416_12.5i_qd_mlok_handguard</t>
+  </si>
+  <si>
+    <t>kf_416_11.5i_qd_mlok_handguard</t>
+  </si>
+  <si>
+    <t>Standard Length Quad Rail</t>
+  </si>
+  <si>
+    <t>Extended Length Quad Rail</t>
+  </si>
+  <si>
+    <t>DMR Extra Long</t>
+  </si>
+  <si>
+    <t>9" Quad Rail</t>
+  </si>
+  <si>
+    <t>9" Quad Rail w/ Flip Up Sight</t>
+  </si>
+  <si>
+    <t>KF416C</t>
+  </si>
+  <si>
+    <t>KF416 Short H-Key</t>
+  </si>
+  <si>
+    <t>KF416 Long QD H-Key</t>
+  </si>
+  <si>
+    <t>KF416 11.5" QD MLOK</t>
+  </si>
+  <si>
+    <t>KF416 12.5" QD MLOK</t>
+  </si>
+  <si>
+    <t>KF416 14.5" QD MLOK</t>
   </si>
 </sst>
 </file>
@@ -585,9 +627,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -647,9 +688,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -687,7 +728,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -793,7 +834,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -935,7 +976,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -943,354 +984,468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>0.28000000000000003</v>
+        <v>0.26</v>
       </c>
       <c r="E3">
+        <v>-9</v>
+      </c>
+      <c r="F3">
         <v>-10</v>
       </c>
-      <c r="F3">
+      <c r="M3">
+        <v>1000</v>
+      </c>
+      <c r="N3">
+        <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
+        <v>19</v>
+      </c>
+      <c r="P3">
+        <v>124</v>
+      </c>
+      <c r="Q3">
+        <v>0.03</v>
+      </c>
+      <c r="R3">
+        <f>P3*0.0013+0.07+Q3</f>
+        <v>0.26119999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>0.31</v>
+      </c>
+      <c r="E4">
+        <v>-10</v>
+      </c>
+      <c r="F4">
         <v>-14</v>
       </c>
-      <c r="M3">
+      <c r="M4">
         <v>0</v>
       </c>
-      <c r="N3" s="1">
-        <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
-        <v>18.799999999999997</v>
+      <c r="N4">
+        <f t="shared" ref="N4:N13" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
+        <v>19.200000000000003</v>
+      </c>
+      <c r="P4">
+        <v>160</v>
+      </c>
+      <c r="Q4">
+        <v>0.03</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4:R13" si="1">P4*0.0013+0.07+Q4</f>
+        <v>0.30800000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>0.36</v>
-      </c>
-      <c r="E4">
-        <v>-11</v>
-      </c>
-      <c r="F4">
-        <v>-18</v>
-      </c>
-      <c r="M4">
-        <v>750</v>
-      </c>
-      <c r="N4" s="1">
-        <f>C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
-        <v>17.399999999999999</v>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>0.34</v>
+      </c>
+      <c r="E5">
+        <v>-12</v>
+      </c>
+      <c r="F5">
+        <v>-16</v>
+      </c>
+      <c r="M5">
+        <v>500</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="P5">
+        <v>187</v>
+      </c>
+      <c r="Q5">
+        <v>0.03</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="1"/>
+        <v>0.34309999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>0.25</v>
-      </c>
-      <c r="E5">
-        <v>-9</v>
-      </c>
-      <c r="F5">
-        <v>-10</v>
-      </c>
-      <c r="M5">
-        <v>900</v>
-      </c>
-      <c r="N5" s="1">
-        <f>C5-D5*20-E5*0.8-F5*0.6-H5*5+I5*10+J5/300</f>
-        <v>19.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>0.34</v>
+        <v>0.43</v>
       </c>
       <c r="E6">
-        <v>-12</v>
+        <v>-15</v>
       </c>
       <c r="F6">
         <v>-15</v>
       </c>
       <c r="M6">
-        <v>1400</v>
-      </c>
-      <c r="N6" s="1">
-        <f t="shared" ref="N6" si="0">C6-D6*20-E6*0.8-F6*0.6-H6*5+I6*10+J6/300</f>
-        <v>18.8</v>
+        <v>1000</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="P6">
+        <v>255</v>
+      </c>
+      <c r="Q6">
+        <v>0.03</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="1"/>
+        <v>0.43149999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N7" s="1"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>0.32</v>
+      </c>
+      <c r="E7">
+        <v>-12</v>
+      </c>
+      <c r="F7">
+        <v>-14</v>
+      </c>
+      <c r="M7">
+        <v>500</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="P7">
+        <v>170</v>
+      </c>
+      <c r="Q7">
+        <v>0.03</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>0.32100000000000006</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N8" s="1"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>0.33</v>
+      </c>
+      <c r="E8">
+        <v>-12</v>
+      </c>
+      <c r="F8">
+        <v>-14</v>
+      </c>
+      <c r="M8">
+        <v>750</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="P8">
+        <v>170</v>
+      </c>
+      <c r="Q8">
+        <v>0.04</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>0.33100000000000002</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N9" s="1"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>0.3</v>
+      </c>
+      <c r="E9">
+        <v>-9</v>
+      </c>
+      <c r="F9">
+        <v>-16</v>
+      </c>
+      <c r="M9">
+        <v>1000</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>19.799999999999997</v>
+      </c>
+      <c r="P9">
+        <v>166</v>
+      </c>
+      <c r="Q9">
+        <v>0.01</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>0.29580000000000001</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N10" s="1"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>0.38</v>
+      </c>
+      <c r="E10">
+        <v>-12</v>
+      </c>
+      <c r="F10">
+        <v>-19</v>
+      </c>
+      <c r="M10">
+        <v>1500</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>19.400000000000002</v>
+      </c>
+      <c r="P10">
+        <v>234</v>
+      </c>
+      <c r="Q10">
+        <v>0.01</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>0.38419999999999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N11" s="1"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0.3</v>
+      </c>
+      <c r="E11">
+        <v>-13</v>
+      </c>
+      <c r="F11">
+        <v>-9</v>
+      </c>
+      <c r="M11">
+        <v>1000</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>19.8</v>
+      </c>
+      <c r="P11">
+        <v>176</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>0.29880000000000001</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N12" s="1"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>0.32</v>
+      </c>
+      <c r="E12">
+        <v>-14</v>
+      </c>
+      <c r="F12">
+        <v>-10</v>
+      </c>
+      <c r="M12">
+        <v>1250</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>19.8</v>
+      </c>
+      <c r="P12">
+        <f>195</f>
+        <v>195</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>0.32350000000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N49" s="1"/>
-    </row>
-    <row r="50" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N55" s="1"/>
-    </row>
-    <row r="56" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N57" s="1"/>
-    </row>
-    <row r="58" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N58" s="1"/>
-    </row>
-    <row r="59" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N59" s="1"/>
-    </row>
-    <row r="60" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N61" s="1"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>0.37</v>
+      </c>
+      <c r="E13">
+        <v>-16</v>
+      </c>
+      <c r="F13">
+        <v>-12</v>
+      </c>
+      <c r="M13">
+        <v>1500</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="P13">
+        <v>233</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>0.37290000000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>